<commit_message>
Older adult data and cvoe poster
</commit_message>
<xml_diff>
--- a/CVOE/1 Analysis/updated means 4_16_19.xlsx
+++ b/CVOE/1 Analysis/updated means 4_16_19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm\OneDrive\Documents\GitHub\Spring-2019-Projects\CVOE\1 Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{A60D5FAB-7B4F-4A67-A014-1F017F838D85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1CD1173F-7802-44E7-84CB-7EA6EEA0A161}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="8_{A60D5FAB-7B4F-4A67-A014-1F017F838D85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{85C4A235-DF1E-408B-A472-80B1989757E1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5748" xr2:uid="{C35E88EF-7609-4E8C-927F-27517DDDB189}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Sub</t>
   </si>
@@ -96,6 +96,30 @@
   </si>
   <si>
     <t>Rand Nonsw RT</t>
+  </si>
+  <si>
+    <t>non-switch</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>upper 95%</t>
+  </si>
+  <si>
+    <t>lower 95%</t>
+  </si>
+  <si>
+    <t>Global Switch</t>
+  </si>
+  <si>
+    <t>Local Switch</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Local</t>
   </si>
 </sst>
 </file>
@@ -163,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -172,6 +196,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +511,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E856CAE-B9E9-46DD-BE19-328072D1CF91}">
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="AF3" sqref="AF3:AG31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +525,7 @@
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,41 +562,65 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -606,42 +657,74 @@
       <c r="L2">
         <v>273.09433962264097</v>
       </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M13" si="0">(F2 + H2) / 2</f>
+        <v>1366.3818181818201</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N13" si="1">(G2 + I2) / 2</f>
+        <v>1091.1936078761792</v>
+      </c>
       <c r="O2">
+        <f>(I2 + J2) /2</f>
+        <v>542.91105794789996</v>
+      </c>
+      <c r="P2">
+        <f>(K2 + L2) /2</f>
+        <v>113.55214408233243</v>
+      </c>
+      <c r="S2">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P2">
+      <c r="T2">
         <v>5.2631578947368501E-2</v>
       </c>
-      <c r="Q2">
-        <f>AVERAGE(O2:P2)</f>
+      <c r="U2">
+        <f>AVERAGE(S2:T2)</f>
         <v>3.1524122807017552E-2</v>
       </c>
-      <c r="R2">
+      <c r="V2">
         <v>7.2727272727272793E-2</v>
       </c>
-      <c r="S2">
+      <c r="W2">
         <v>7.0175438596491196E-2</v>
       </c>
-      <c r="T2">
+      <c r="X2">
         <v>1.85185185185185E-2</v>
       </c>
-      <c r="U2">
+      <c r="Y2">
         <v>0</v>
       </c>
-      <c r="V2">
+      <c r="Z2">
         <v>3.86513157894737E-2</v>
       </c>
-      <c r="W2">
+      <c r="AA2">
         <v>-3.15241228070176E-2</v>
       </c>
-      <c r="X2">
+      <c r="AB2">
         <v>2.5518341307815299E-3</v>
       </c>
-      <c r="Y2">
+      <c r="AC2">
         <v>1.85185185185185E-2</v>
       </c>
+      <c r="AD2">
+        <f>(W2 + Y2) /2</f>
+        <v>3.5087719298245598E-2</v>
+      </c>
+      <c r="AE2">
+        <f t="shared" ref="AE2:AE10" si="2">(V2+X2) /2</f>
+        <v>4.5622895622895648E-2</v>
+      </c>
+      <c r="AF2">
+        <f>(Z2 + AA2) /2</f>
+        <v>3.56359649122805E-3</v>
+      </c>
+      <c r="AG2">
+        <f>(AB2 + AC2) / 2</f>
+        <v>1.0535176324650015E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -678,42 +761,74 @@
       <c r="L3">
         <v>106.090005844535</v>
       </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>971.05932203389852</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="1"/>
+        <v>707.17682726884141</v>
+      </c>
       <c r="O3">
+        <f t="shared" ref="O3:O31" si="3">(I3 + J3) /2</f>
+        <v>337.20432665924551</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P31" si="4">(K3 + L3) /2</f>
+        <v>41.56953459042095</v>
+      </c>
+      <c r="S3">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="P3">
+      <c r="T3">
         <v>3.1578947368420998E-2</v>
       </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q20" si="0">AVERAGE(O3:P3)</f>
+      <c r="U3">
+        <f t="shared" ref="U3:U20" si="5">AVERAGE(S3:T3)</f>
         <v>2.6206140350877198E-2</v>
       </c>
-      <c r="R3">
+      <c r="V3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="S3">
+      <c r="W3">
         <v>4.91803278688525E-2</v>
       </c>
-      <c r="T3">
+      <c r="X3">
         <v>3.3898305084745797E-2</v>
       </c>
-      <c r="U3">
+      <c r="Y3">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="V3">
+      <c r="Z3">
         <v>2.2974187517975302E-2</v>
       </c>
-      <c r="W3">
+      <c r="AA3">
         <v>6.5807448950244698E-3</v>
       </c>
-      <c r="X3">
+      <c r="AB3">
         <v>-2.4180327868852498E-2</v>
       </c>
-      <c r="Y3">
+      <c r="AC3">
         <v>1.1114198388441101E-3</v>
       </c>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD31" si="6">(W3 + Y3) /2</f>
+        <v>4.0983606557377095E-2</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" si="2"/>
+        <v>2.9449152542372899E-2</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" ref="AF3:AF31" si="7">(Z3 + AA3) /2</f>
+        <v>1.4777466206499886E-2</v>
+      </c>
+      <c r="AG3">
+        <f t="shared" ref="AG3:AG31" si="8">(AB3 + AC3) / 2</f>
+        <v>-1.1534454015004194E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -750,42 +865,74 @@
       <c r="L4">
         <v>198.053333333333</v>
       </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>1352.1481481481501</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>1133.6570611916266</v>
+      </c>
       <c r="O4">
+        <f t="shared" si="3"/>
+        <v>717.11264090177156</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="4"/>
+        <v>105.54204053109704</v>
+      </c>
+      <c r="S4">
         <v>5.2631578947368501E-2</v>
       </c>
-      <c r="P4">
+      <c r="T4">
         <v>4.1666666666666602E-2</v>
       </c>
-      <c r="Q4">
-        <f t="shared" si="0"/>
+      <c r="U4">
+        <f t="shared" si="5"/>
         <v>4.7149122807017552E-2</v>
       </c>
-      <c r="R4">
+      <c r="V4">
         <v>0.10344827586206901</v>
       </c>
-      <c r="S4">
+      <c r="W4">
         <v>0.16666666666666699</v>
       </c>
-      <c r="T4">
+      <c r="X4">
         <v>0.101694915254237</v>
       </c>
-      <c r="U4">
+      <c r="Y4">
         <v>6.8965517241379296E-2</v>
       </c>
-      <c r="V4">
+      <c r="Z4">
         <v>0.11951754385964899</v>
       </c>
-      <c r="W4">
+      <c r="AA4">
         <v>2.1816394434361799E-2</v>
       </c>
-      <c r="X4">
+      <c r="AB4">
         <v>-6.3218390804597693E-2</v>
       </c>
-      <c r="Y4">
+      <c r="AC4">
         <v>3.2729398012857902E-2</v>
       </c>
+      <c r="AD4">
+        <f t="shared" si="6"/>
+        <v>0.11781609195402315</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="2"/>
+        <v>0.10257159555815301</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" si="7"/>
+        <v>7.0666969147005404E-2</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" si="8"/>
+        <v>-1.5244496395869896E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -822,42 +969,74 @@
       <c r="L5">
         <v>147.957334891876</v>
       </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>1570.987434248975</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>1244.629665524704</v>
+      </c>
       <c r="O5">
+        <f t="shared" si="3"/>
+        <v>770.31456190855147</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="4"/>
+        <v>122.6905318527177</v>
+      </c>
+      <c r="S5">
         <v>0</v>
       </c>
-      <c r="P5">
+      <c r="T5">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="Q5">
-        <f t="shared" si="0"/>
+      <c r="U5">
+        <f t="shared" si="5"/>
         <v>1.0416666666666701E-2</v>
       </c>
-      <c r="R5">
+      <c r="V5">
         <v>1.6806722689075699E-2</v>
       </c>
-      <c r="S5">
+      <c r="W5">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="T5">
+      <c r="X5">
         <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>2.2370218579235001E-2</v>
-      </c>
-      <c r="W5">
-        <v>-1.0416666666666701E-2</v>
-      </c>
-      <c r="X5">
-        <v>-1.5980162556826001E-2</v>
       </c>
       <c r="Y5">
         <v>0</v>
       </c>
+      <c r="Z5">
+        <v>2.2370218579235001E-2</v>
+      </c>
+      <c r="AA5">
+        <v>-1.0416666666666701E-2</v>
+      </c>
+      <c r="AB5">
+        <v>-1.5980162556826001E-2</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="6"/>
+        <v>1.6393442622950848E-2</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="2"/>
+        <v>8.4033613445378495E-3</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="7"/>
+        <v>5.9767759562841501E-3</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="8"/>
+        <v>-7.9900812784130006E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -894,42 +1073,74 @@
       <c r="L6">
         <v>35.203246753247001</v>
       </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>1248.5267857142849</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>906.82168255132058</v>
+      </c>
       <c r="O6">
-        <v>8.3333333333333398E-2</v>
+        <f t="shared" si="3"/>
+        <v>529.91333263510649</v>
       </c>
       <c r="P6">
-        <v>3.125E-2</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="0"/>
-        <v>5.7291666666666699E-2</v>
-      </c>
-      <c r="R6">
-        <v>6.7226890756302504E-2</v>
+        <f t="shared" si="4"/>
+        <v>26.682991301151802</v>
       </c>
       <c r="S6">
         <v>8.3333333333333398E-2</v>
       </c>
       <c r="T6">
+        <v>3.125E-2</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="5"/>
+        <v>5.7291666666666699E-2</v>
+      </c>
+      <c r="V6">
+        <v>6.7226890756302504E-2</v>
+      </c>
+      <c r="W6">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="X6">
         <v>0.101694915254237</v>
       </c>
-      <c r="U6">
+      <c r="Y6">
         <v>6.6666666666666693E-2</v>
       </c>
-      <c r="V6">
+      <c r="Z6">
         <v>2.6041666666666699E-2</v>
       </c>
-      <c r="W6">
+      <c r="AA6">
         <v>9.3749999999999702E-3</v>
       </c>
-      <c r="X6">
+      <c r="AB6">
         <v>-1.6106442577030901E-2</v>
       </c>
-      <c r="Y6">
+      <c r="AC6">
         <v>3.5028248587570601E-2</v>
       </c>
+      <c r="AD6">
+        <f t="shared" si="6"/>
+        <v>7.5000000000000039E-2</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="2"/>
+        <v>8.4460903005269761E-2</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="7"/>
+        <v>1.7708333333333333E-2</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="8"/>
+        <v>9.4609030052698502E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -966,42 +1177,74 @@
       <c r="L7">
         <v>463.09649122807002</v>
       </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>1262.605263157895</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>1038.1836792134779</v>
+      </c>
       <c r="O7">
+        <f t="shared" si="3"/>
+        <v>350.665604040988</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>388.66897926634749</v>
+      </c>
+      <c r="S7">
         <v>1.05263157894737E-2</v>
       </c>
-      <c r="P7">
+      <c r="T7">
         <v>2.1052631578947299E-2</v>
       </c>
-      <c r="Q7">
-        <f t="shared" si="0"/>
+      <c r="U7">
+        <f t="shared" si="5"/>
         <v>1.5789473684210499E-2</v>
       </c>
-      <c r="R7">
+      <c r="V7">
         <v>8.9285714285714003E-3</v>
       </c>
-      <c r="S7">
+      <c r="W7">
         <v>0</v>
       </c>
-      <c r="T7">
+      <c r="X7">
         <v>0</v>
       </c>
-      <c r="U7">
+      <c r="Y7">
         <v>0.05</v>
       </c>
-      <c r="V7">
+      <c r="Z7">
         <v>-1.5789473684210499E-2</v>
       </c>
-      <c r="W7">
+      <c r="AA7">
         <v>3.4210526315789497E-2</v>
       </c>
-      <c r="X7">
+      <c r="AB7">
         <v>8.9285714285714003E-3</v>
       </c>
-      <c r="Y7">
+      <c r="AC7">
         <v>-0.05</v>
       </c>
+      <c r="AD7">
+        <f t="shared" si="6"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="2"/>
+        <v>4.4642857142857002E-3</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="7"/>
+        <v>9.2105263157894988E-3</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="8"/>
+        <v>-2.0535714285714303E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1038,42 +1281,74 @@
       <c r="L8">
         <v>369.36238244514101</v>
       </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>1580.722958397535</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>1391.1417415318701</v>
+      </c>
       <c r="O8">
+        <f t="shared" si="3"/>
+        <v>832.19814222106606</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>123.112609929413</v>
+      </c>
+      <c r="S8">
         <v>0</v>
       </c>
-      <c r="P8">
+      <c r="T8">
         <v>0.105263157894737</v>
       </c>
-      <c r="Q8">
-        <f t="shared" si="0"/>
+      <c r="U8">
+        <f t="shared" si="5"/>
         <v>5.2631578947368501E-2</v>
       </c>
-      <c r="R8">
+      <c r="V8">
         <v>3.3898305084745797E-2</v>
       </c>
-      <c r="S8">
+      <c r="W8">
         <v>3.3333333333333298E-2</v>
       </c>
-      <c r="T8">
+      <c r="X8">
         <v>8.4745762711864403E-2</v>
       </c>
-      <c r="U8">
+      <c r="Y8">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="V8">
+      <c r="Z8">
         <v>-1.9298245614035099E-2</v>
       </c>
-      <c r="W8">
+      <c r="AA8">
         <v>-3.59649122807017E-2</v>
       </c>
-      <c r="X8">
+      <c r="AB8">
         <v>5.6497175141245705E-4</v>
       </c>
-      <c r="Y8">
+      <c r="AC8">
         <v>6.8079096045197698E-2</v>
       </c>
+      <c r="AD8">
+        <f t="shared" si="6"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="2"/>
+        <v>5.93220338983051E-2</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="7"/>
+        <v>-2.7631578947368399E-2</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="8"/>
+        <v>3.4322033898305078E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1110,42 +1385,74 @@
       <c r="L9">
         <v>121.049745618994</v>
       </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>1558.53591954023</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>1197.4048712970971</v>
+      </c>
       <c r="O9">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>715.22407743496706</v>
       </c>
       <c r="P9">
-        <v>1.04166666666666E-2</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="0"/>
-        <v>5.2083333333333001E-3</v>
-      </c>
-      <c r="R9">
-        <v>8.3333333333333003E-3</v>
+        <f t="shared" si="4"/>
+        <v>149.3074485670725</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9">
+        <v>1.04166666666666E-2</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="5"/>
+        <v>5.2083333333333001E-3</v>
+      </c>
+      <c r="V9">
+        <v>8.3333333333333003E-3</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
         <v>5.1724137931034503E-2</v>
       </c>
-      <c r="U9">
+      <c r="Y9">
         <v>1.63934426229508E-2</v>
       </c>
-      <c r="V9">
+      <c r="Z9">
         <v>-5.2083333333333096E-3</v>
       </c>
-      <c r="W9">
+      <c r="AA9">
         <v>1.11851092896175E-2</v>
       </c>
-      <c r="X9">
+      <c r="AB9">
         <v>8.3333333333333003E-3</v>
       </c>
-      <c r="Y9">
+      <c r="AC9">
         <v>3.5330695308083603E-2</v>
       </c>
+      <c r="AD9">
+        <f t="shared" si="6"/>
+        <v>8.1967213114753999E-3</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="2"/>
+        <v>3.0028735632183903E-2</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="7"/>
+        <v>2.9883879781420954E-3</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="8"/>
+        <v>2.183201432070845E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1182,42 +1489,74 @@
       <c r="L10">
         <v>17.694915254237198</v>
       </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>1083.5976660183351</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>825.24466004655494</v>
+      </c>
       <c r="O10">
+        <f t="shared" si="3"/>
+        <v>549.19673882053598</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>31.875156892240149</v>
+      </c>
+      <c r="S10">
         <v>0</v>
       </c>
-      <c r="P10">
+      <c r="T10">
         <v>5.2083333333333398E-2</v>
       </c>
-      <c r="Q10">
-        <f t="shared" si="0"/>
+      <c r="U10">
+        <f t="shared" si="5"/>
         <v>2.6041666666666699E-2</v>
       </c>
-      <c r="R10">
+      <c r="V10">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="S10">
+      <c r="W10">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="T10">
+      <c r="X10">
         <v>1.6949152542372801E-2</v>
       </c>
-      <c r="U10">
+      <c r="Y10">
         <v>0</v>
       </c>
-      <c r="V10">
+      <c r="Z10">
         <v>6.7452185792349897E-3</v>
       </c>
-      <c r="W10">
+      <c r="AA10">
         <v>-2.6041666666666699E-2</v>
       </c>
-      <c r="X10">
+      <c r="AB10">
         <v>-1.6120218579234999E-2</v>
       </c>
-      <c r="Y10">
+      <c r="AC10">
         <v>1.6949152542372801E-2</v>
       </c>
+      <c r="AD10">
+        <f t="shared" si="6"/>
+        <v>1.6393442622950848E-2</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="2"/>
+        <v>1.680790960451975E-2</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="7"/>
+        <v>-9.6482240437158542E-3</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="8"/>
+        <v>4.144669815689013E-4</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1254,42 +1593,74 @@
       <c r="L11">
         <v>498.92952127659601</v>
       </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>1959.7751225490199</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>1645.5879170651176</v>
+      </c>
       <c r="O11">
+        <f t="shared" si="3"/>
+        <v>832.47119030461545</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>115.70685747703351</v>
+      </c>
+      <c r="S11">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P11">
+      <c r="T11">
         <v>2.2471910112359599E-2</v>
       </c>
-      <c r="Q11">
-        <f t="shared" si="0"/>
+      <c r="U11">
+        <f t="shared" si="5"/>
         <v>1.64442883895131E-2</v>
       </c>
-      <c r="R11">
+      <c r="V11">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="S11">
+      <c r="W11">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="T11">
+      <c r="X11">
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="U11">
+      <c r="Y11">
         <v>0</v>
       </c>
-      <c r="V11">
+      <c r="Z11">
         <v>4.3890449438202502E-3</v>
       </c>
-      <c r="W11">
+      <c r="AA11">
         <v>-1.64442883895131E-2</v>
       </c>
-      <c r="X11">
+      <c r="AB11">
         <v>-1.0416666666666701E-2</v>
       </c>
-      <c r="Y11">
+      <c r="AC11">
         <v>1.9607843137254902E-2</v>
       </c>
+      <c r="AD11">
+        <f t="shared" si="6"/>
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" ref="AE11:AE13" si="9">(V11+X11) /2</f>
+        <v>1.5012254901960752E-2</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="7"/>
+        <v>-6.0276217228464254E-3</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="8"/>
+        <v>4.5955882352941005E-3</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1326,42 +1697,74 @@
       <c r="L12">
         <v>84.021570319240695</v>
       </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>1044.5664585191794</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>736.70423105312739</v>
+      </c>
       <c r="O12">
+        <f t="shared" si="3"/>
+        <v>344.82043326783503</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>109.23243916312686</v>
+      </c>
+      <c r="S12">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="P12">
+      <c r="T12">
         <v>5.2083333333333398E-2</v>
       </c>
-      <c r="Q12">
-        <f t="shared" si="0"/>
+      <c r="U12">
+        <f t="shared" si="5"/>
         <v>3.6458333333333398E-2</v>
       </c>
-      <c r="R12">
+      <c r="V12">
         <v>8.4033613445377905E-3</v>
       </c>
-      <c r="S12">
+      <c r="W12">
         <v>0</v>
       </c>
-      <c r="T12">
+      <c r="X12">
         <v>1.6949152542372801E-2</v>
       </c>
-      <c r="U12">
+      <c r="Y12">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="V12">
+      <c r="Z12">
         <v>-3.6458333333333398E-2</v>
       </c>
-      <c r="W12">
+      <c r="AA12">
         <v>-1.97916666666667E-2</v>
       </c>
-      <c r="X12">
+      <c r="AB12">
         <v>8.4033613445377905E-3</v>
       </c>
-      <c r="Y12">
+      <c r="AC12">
         <v>2.8248587570611799E-4</v>
       </c>
+      <c r="AD12">
+        <f t="shared" si="6"/>
+        <v>8.3333333333333506E-3</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="9"/>
+        <v>1.2676256943455297E-2</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="7"/>
+        <v>-2.8125000000000049E-2</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="8"/>
+        <v>4.3429236101219541E-3</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1398,42 +1801,74 @@
       <c r="L13">
         <v>193.08771929824599</v>
       </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>1105.08681185723</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>889.98717011874703</v>
+      </c>
       <c r="O13">
+        <f t="shared" si="3"/>
+        <v>481.799809082021</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>126.3403497969063</v>
+      </c>
+      <c r="S13">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="P13">
+      <c r="T13">
         <v>4.1666666666666602E-2</v>
       </c>
-      <c r="Q13">
-        <f t="shared" si="0"/>
+      <c r="U13">
+        <f t="shared" si="5"/>
         <v>3.125E-2</v>
       </c>
-      <c r="R13">
+      <c r="V13">
         <v>2.5641025641025699E-2</v>
       </c>
-      <c r="S13">
+      <c r="W13">
         <v>0.05</v>
       </c>
-      <c r="T13">
+      <c r="X13">
         <v>5.0847457627118599E-2</v>
       </c>
-      <c r="U13">
+      <c r="Y13">
         <v>3.3333333333333298E-2</v>
       </c>
-      <c r="V13">
+      <c r="Z13">
         <v>1.8749999999999999E-2</v>
       </c>
-      <c r="W13">
+      <c r="AA13">
         <v>2.0833333333333298E-3</v>
       </c>
-      <c r="X13">
+      <c r="AB13">
         <v>-2.4358974358974401E-2</v>
       </c>
-      <c r="Y13">
+      <c r="AC13">
         <v>1.7514124293785301E-2</v>
       </c>
+      <c r="AD13">
+        <f t="shared" si="6"/>
+        <v>4.166666666666665E-2</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="9"/>
+        <v>3.8244241634072147E-2</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="7"/>
+        <v>1.0416666666666664E-2</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="8"/>
+        <v>-3.4224250325945501E-3</v>
+      </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1470,42 +1905,74 @@
       <c r="L14">
         <v>160.207471264368</v>
       </c>
+      <c r="M14">
+        <f>(F14 + H14) / 2</f>
+        <v>1536.0086206896549</v>
+      </c>
+      <c r="N14">
+        <f>(E14 + G14)</f>
+        <v>3340.2764367816098</v>
+      </c>
       <c r="O14">
+        <f t="shared" si="3"/>
+        <v>807.99837432907304</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>134.12959770114949</v>
+      </c>
+      <c r="S14">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P14">
+      <c r="T14">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="Q14">
-        <f t="shared" si="0"/>
+      <c r="U14">
+        <f t="shared" si="5"/>
         <v>1.5625E-2</v>
       </c>
-      <c r="R14">
+      <c r="V14">
         <v>8.4033613445377905E-3</v>
       </c>
-      <c r="S14">
+      <c r="W14">
         <v>1.63934426229508E-2</v>
       </c>
-      <c r="T14">
+      <c r="X14">
         <v>1.6949152542372801E-2</v>
       </c>
-      <c r="U14">
+      <c r="Y14">
         <v>3.3333333333333298E-2</v>
       </c>
-      <c r="V14">
+      <c r="Z14">
         <v>7.6844262295083798E-4</v>
       </c>
-      <c r="W14">
+      <c r="AA14">
         <v>1.7708333333333302E-2</v>
       </c>
-      <c r="X14">
+      <c r="AB14">
         <v>-7.9900812784130509E-3</v>
       </c>
-      <c r="Y14">
+      <c r="AC14">
         <v>-1.63841807909605E-2</v>
       </c>
+      <c r="AD14">
+        <f t="shared" si="6"/>
+        <v>2.4863387978142047E-2</v>
+      </c>
+      <c r="AE14">
+        <f>(V14+X14) /2</f>
+        <v>1.2676256943455297E-2</v>
+      </c>
+      <c r="AF14">
+        <f t="shared" si="7"/>
+        <v>9.2383879781420698E-3</v>
+      </c>
+      <c r="AG14">
+        <f t="shared" si="8"/>
+        <v>-1.2187131034686775E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1542,42 +2009,74 @@
       <c r="L15">
         <v>173.90658307210001</v>
       </c>
+      <c r="M15">
+        <f t="shared" ref="M15:M31" si="10">(F15 + H15) / 2</f>
+        <v>1417.59601275917</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ref="N15:N31" si="11">(E15 + G15)</f>
+        <v>3061.52476489028</v>
+      </c>
       <c r="O15">
+        <f t="shared" si="3"/>
+        <v>610.46839532849754</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>113.1663696859703</v>
+      </c>
+      <c r="S15">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P15">
+      <c r="T15">
         <v>3.125E-2</v>
       </c>
-      <c r="Q15">
-        <f t="shared" si="0"/>
+      <c r="U15">
+        <f t="shared" si="5"/>
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="R15">
+      <c r="V15">
         <v>3.4188034188034198E-2</v>
       </c>
-      <c r="S15">
+      <c r="W15">
         <v>4.91803278688525E-2</v>
       </c>
-      <c r="T15">
+      <c r="X15">
         <v>5.1724137931034503E-2</v>
       </c>
-      <c r="U15">
+      <c r="Y15">
         <v>0</v>
       </c>
-      <c r="V15">
+      <c r="Z15">
         <v>2.8346994535519199E-2</v>
       </c>
-      <c r="W15">
+      <c r="AA15">
         <v>-2.0833333333333301E-2</v>
       </c>
-      <c r="X15">
+      <c r="AB15">
         <v>-1.49922936808183E-2</v>
       </c>
-      <c r="Y15">
+      <c r="AC15">
         <v>5.1724137931034503E-2</v>
       </c>
+      <c r="AD15">
+        <f t="shared" si="6"/>
+        <v>2.459016393442625E-2</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" ref="AE15:AE31" si="12">(V15+X15) /2</f>
+        <v>4.2956086059534354E-2</v>
+      </c>
+      <c r="AF15">
+        <f t="shared" si="7"/>
+        <v>3.7568306010929489E-3</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="8"/>
+        <v>1.8365922125108101E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1614,33 +2113,37 @@
       <c r="L16">
         <v>362.26297169811301</v>
       </c>
+      <c r="M16">
+        <f t="shared" si="10"/>
+        <v>2271.3773584905703</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="11"/>
+        <v>4900.0336538461497</v>
+      </c>
       <c r="O16">
+        <f t="shared" si="3"/>
+        <v>1335.9111608241301</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>178.63946843251074</v>
+      </c>
+      <c r="S16">
         <v>1.0638297872340399E-2</v>
       </c>
-      <c r="P16">
+      <c r="T16">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="Q16">
-        <f t="shared" si="0"/>
+      <c r="U16">
+        <f t="shared" si="5"/>
         <v>1.5735815602836899E-2</v>
       </c>
-      <c r="R16">
+      <c r="V16">
         <v>0</v>
       </c>
-      <c r="S16">
+      <c r="W16">
         <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>-1.5735815602836899E-2</v>
-      </c>
-      <c r="W16">
-        <v>-1.5735815602836899E-2</v>
       </c>
       <c r="X16">
         <v>0</v>
@@ -1648,8 +2151,36 @@
       <c r="Y16">
         <v>0</v>
       </c>
+      <c r="Z16">
+        <v>-1.5735815602836899E-2</v>
+      </c>
+      <c r="AA16">
+        <v>-1.5735815602836899E-2</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <f t="shared" si="7"/>
+        <v>-1.5735815602836899E-2</v>
+      </c>
+      <c r="AG16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1686,42 +2217,74 @@
       <c r="L17">
         <v>498.85272727272701</v>
       </c>
+      <c r="M17">
+        <f t="shared" si="10"/>
+        <v>1493.30092449923</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="11"/>
+        <v>3689.2890909090902</v>
+      </c>
       <c r="O17">
+        <f t="shared" si="3"/>
+        <v>947.58627980544554</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="4"/>
+        <v>351.34362095531549</v>
+      </c>
+      <c r="S17">
         <v>3.125E-2</v>
       </c>
-      <c r="P17">
+      <c r="T17">
         <v>4.1666666666666602E-2</v>
       </c>
-      <c r="Q17">
-        <f t="shared" si="0"/>
+      <c r="U17">
+        <f t="shared" si="5"/>
         <v>3.6458333333333301E-2</v>
       </c>
-      <c r="R17">
+      <c r="V17">
         <v>5.4054054054054099E-2</v>
       </c>
-      <c r="S17">
+      <c r="W17">
         <v>0.107142857142857</v>
       </c>
-      <c r="T17">
+      <c r="X17">
         <v>5.1724137931034503E-2</v>
       </c>
-      <c r="U17">
+      <c r="Y17">
         <v>1.63934426229508E-2</v>
       </c>
-      <c r="V17">
+      <c r="Z17">
         <v>7.0684523809523794E-2</v>
       </c>
-      <c r="W17">
+      <c r="AA17">
         <v>-2.0064890710382501E-2</v>
       </c>
-      <c r="X17">
+      <c r="AB17">
         <v>-5.3088803088802997E-2</v>
       </c>
-      <c r="Y17">
+      <c r="AC17">
         <v>3.5330695308083603E-2</v>
       </c>
+      <c r="AD17">
+        <f t="shared" si="6"/>
+        <v>6.1768149882903897E-2</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="12"/>
+        <v>5.2889095992544301E-2</v>
+      </c>
+      <c r="AF17">
+        <f t="shared" si="7"/>
+        <v>2.5309816549570645E-2</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" si="8"/>
+        <v>-8.879053890359697E-3</v>
+      </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>19</v>
       </c>
@@ -1758,42 +2321,74 @@
       <c r="L18">
         <v>30.5477207977208</v>
       </c>
+      <c r="M18">
+        <f t="shared" si="10"/>
+        <v>1261.539861895795</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="11"/>
+        <v>2524.3066433566401</v>
+      </c>
       <c r="O18">
+        <f t="shared" si="3"/>
+        <v>503.81022802851749</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="4"/>
+        <v>0.61345978252760069</v>
+      </c>
+      <c r="S18">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P18">
+      <c r="T18">
         <v>4.1666666666666602E-2</v>
       </c>
-      <c r="Q18">
-        <f t="shared" si="0"/>
+      <c r="U18">
+        <f t="shared" si="5"/>
         <v>2.6041666666666602E-2</v>
       </c>
-      <c r="R18">
+      <c r="V18">
         <v>0.108333333333333</v>
       </c>
-      <c r="S18">
+      <c r="W18">
         <v>0.14754098360655701</v>
       </c>
-      <c r="T18">
+      <c r="X18">
         <v>6.7796610169491595E-2</v>
       </c>
-      <c r="U18">
+      <c r="Y18">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="V18">
+      <c r="Z18">
         <v>0.12149931693989099</v>
       </c>
-      <c r="W18">
+      <c r="AA18">
         <v>6.7452185792350504E-3</v>
       </c>
-      <c r="X18">
+      <c r="AB18">
         <v>-3.92076502732241E-2</v>
       </c>
-      <c r="Y18">
+      <c r="AC18">
         <v>3.5009724923589898E-2</v>
       </c>
+      <c r="AD18">
+        <f t="shared" si="6"/>
+        <v>9.0163934426229358E-2</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="12"/>
+        <v>8.8064971751412299E-2</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="7"/>
+        <v>6.412226775956302E-2</v>
+      </c>
+      <c r="AG18">
+        <f t="shared" si="8"/>
+        <v>-2.0989626748171009E-3</v>
+      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>20</v>
       </c>
@@ -1830,42 +2425,74 @@
       <c r="L19">
         <v>137.339184952978</v>
       </c>
+      <c r="M19">
+        <f t="shared" si="10"/>
+        <v>1440.6712121212099</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="11"/>
+        <v>3119.0197044335</v>
+      </c>
       <c r="O19">
+        <f t="shared" si="3"/>
+        <v>600.046884164223</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="4"/>
+        <v>118.8386400955365</v>
+      </c>
+      <c r="S19">
         <v>0</v>
       </c>
-      <c r="P19">
+      <c r="T19">
         <v>3.125E-2</v>
       </c>
-      <c r="Q19">
-        <f t="shared" si="0"/>
+      <c r="U19">
+        <f t="shared" si="5"/>
         <v>1.5625E-2</v>
       </c>
-      <c r="R19">
+      <c r="V19">
         <v>4.2372881355932202E-2</v>
       </c>
-      <c r="S19">
+      <c r="W19">
         <v>3.3333333333333298E-2</v>
       </c>
-      <c r="T19">
+      <c r="X19">
         <v>5.0847457627118599E-2</v>
       </c>
-      <c r="U19">
+      <c r="Y19">
         <v>1.63934426229508E-2</v>
       </c>
-      <c r="V19">
+      <c r="Z19">
         <v>1.7708333333333302E-2</v>
       </c>
-      <c r="W19">
+      <c r="AA19">
         <v>7.6844262295083798E-4</v>
       </c>
-      <c r="X19">
+      <c r="AB19">
         <v>9.0395480225988808E-3</v>
       </c>
-      <c r="Y19">
+      <c r="AC19">
         <v>3.4454015004167803E-2</v>
       </c>
+      <c r="AD19">
+        <f t="shared" si="6"/>
+        <v>2.4863387978142047E-2</v>
+      </c>
+      <c r="AE19">
+        <f t="shared" si="12"/>
+        <v>4.6610169491525397E-2</v>
+      </c>
+      <c r="AF19">
+        <f t="shared" si="7"/>
+        <v>9.2383879781420698E-3</v>
+      </c>
+      <c r="AG19">
+        <f t="shared" si="8"/>
+        <v>2.1746781513383343E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>21</v>
       </c>
@@ -1902,42 +2529,74 @@
       <c r="L20">
         <v>106.282583284629</v>
       </c>
+      <c r="M20">
+        <f t="shared" si="10"/>
+        <v>996.13879310344998</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="11"/>
+        <v>2183.347011596793</v>
+      </c>
       <c r="O20">
+        <f t="shared" si="3"/>
+        <v>500.79359859543899</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="4"/>
+        <v>95.534712694946052</v>
+      </c>
+      <c r="S20">
         <v>4.1666666666666602E-2</v>
       </c>
-      <c r="P20">
+      <c r="T20">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="Q20">
-        <f t="shared" si="0"/>
+      <c r="U20">
+        <f t="shared" si="5"/>
         <v>2.6041666666666602E-2</v>
       </c>
-      <c r="R20">
+      <c r="V20">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="S20">
+      <c r="W20">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="T20">
+      <c r="X20">
         <v>3.3898305084745797E-2</v>
       </c>
-      <c r="U20">
+      <c r="Y20">
         <v>1.63934426229508E-2</v>
       </c>
-      <c r="V20">
+      <c r="Z20">
         <v>6.7452185792350504E-3</v>
       </c>
-      <c r="W20">
+      <c r="AA20">
         <v>-9.6482240437157901E-3</v>
       </c>
-      <c r="X20">
+      <c r="AB20">
         <v>-7.7868852459016501E-3</v>
       </c>
-      <c r="Y20">
+      <c r="AC20">
         <v>1.75048624617949E-2</v>
       </c>
+      <c r="AD20">
+        <f t="shared" si="6"/>
+        <v>2.459016393442625E-2</v>
+      </c>
+      <c r="AE20">
+        <f t="shared" si="12"/>
+        <v>2.9449152542372899E-2</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="7"/>
+        <v>-1.4515027322403698E-3</v>
+      </c>
+      <c r="AG20">
+        <f t="shared" si="8"/>
+        <v>4.8589886079466252E-3</v>
+      </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>22</v>
       </c>
@@ -1974,41 +2633,73 @@
       <c r="L21">
         <v>160.41873551803999</v>
       </c>
+      <c r="M21">
+        <f t="shared" si="10"/>
+        <v>1527.79912280702</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="11"/>
+        <v>3565.7348382749401</v>
+      </c>
       <c r="O21">
+        <f t="shared" si="3"/>
+        <v>829.21491228070158</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="4"/>
+        <v>255.0682963304485</v>
+      </c>
+      <c r="S21">
         <v>0</v>
       </c>
-      <c r="P21">
+      <c r="T21">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="Q21">
+      <c r="U21">
         <v>5.2083333333333096E-3</v>
       </c>
-      <c r="R21">
+      <c r="V21">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="S21">
+      <c r="W21">
         <v>4.91803278688525E-2</v>
       </c>
-      <c r="T21">
+      <c r="X21">
         <v>5.0847457627118599E-2</v>
       </c>
-      <c r="U21">
+      <c r="Y21">
         <v>0</v>
       </c>
-      <c r="V21">
+      <c r="Z21">
         <v>4.3971994535519199E-2</v>
       </c>
-      <c r="W21">
+      <c r="AA21">
         <v>-5.2083333333333096E-3</v>
       </c>
-      <c r="X21">
+      <c r="AB21">
         <v>-2.4180327868852498E-2</v>
       </c>
-      <c r="Y21">
+      <c r="AC21">
         <v>5.0847457627118599E-2</v>
       </c>
+      <c r="AD21">
+        <f t="shared" si="6"/>
+        <v>2.459016393442625E-2</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" si="12"/>
+        <v>3.79237288135593E-2</v>
+      </c>
+      <c r="AF21">
+        <f t="shared" si="7"/>
+        <v>1.9381830601092945E-2</v>
+      </c>
+      <c r="AG21">
+        <f t="shared" si="8"/>
+        <v>1.333356487913305E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>23</v>
       </c>
@@ -2045,41 +2736,73 @@
       <c r="L22">
         <v>168.12130275839101</v>
       </c>
+      <c r="M22">
+        <f t="shared" si="10"/>
+        <v>954.34364435429347</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="11"/>
+        <v>2355.1416949152499</v>
+      </c>
       <c r="O22">
+        <f t="shared" si="3"/>
+        <v>376.6164188832085</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="4"/>
+        <v>223.22720310333352</v>
+      </c>
+      <c r="S22">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P22">
+      <c r="T22">
         <v>0.15625</v>
       </c>
-      <c r="Q22">
+      <c r="U22">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="R22">
+      <c r="V22">
         <v>8.3333333333333398E-2</v>
       </c>
-      <c r="S22">
+      <c r="W22">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="T22">
+      <c r="X22">
         <v>0.13559322033898299</v>
       </c>
-      <c r="U22">
+      <c r="Y22">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="V22">
+      <c r="Z22">
         <v>-5.0546448087431597E-2</v>
       </c>
-      <c r="W22">
+      <c r="AA22">
         <v>-5.0546448087431597E-2</v>
       </c>
-      <c r="X22">
+      <c r="AB22">
         <v>5.0546448087431702E-2</v>
       </c>
-      <c r="Y22">
+      <c r="AC22">
         <v>0.102806335093081</v>
       </c>
+      <c r="AD22">
+        <f t="shared" si="6"/>
+        <v>3.2786885245901697E-2</v>
+      </c>
+      <c r="AE22">
+        <f t="shared" si="12"/>
+        <v>0.1094632768361582</v>
+      </c>
+      <c r="AF22">
+        <f t="shared" si="7"/>
+        <v>-5.0546448087431597E-2</v>
+      </c>
+      <c r="AG22">
+        <f t="shared" si="8"/>
+        <v>7.6676391590256354E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>24</v>
       </c>
@@ -2116,41 +2839,73 @@
       <c r="L23">
         <v>302.81098382749298</v>
       </c>
+      <c r="M23">
+        <f t="shared" si="10"/>
+        <v>1613.6661117277099</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="11"/>
+        <v>3660.3200549450603</v>
+      </c>
       <c r="O23">
+        <f t="shared" si="3"/>
+        <v>923.5258740367085</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="4"/>
+        <v>216.49391574481749</v>
+      </c>
+      <c r="S23">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P23">
+      <c r="T23">
         <v>3.125E-2</v>
       </c>
-      <c r="Q23">
+      <c r="U23">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="R23">
+      <c r="V23">
         <v>4.1666666666666602E-2</v>
       </c>
-      <c r="S23">
+      <c r="W23">
         <v>4.91803278688525E-2</v>
       </c>
-      <c r="T23">
+      <c r="X23">
         <v>3.3898305084745797E-2</v>
       </c>
-      <c r="U23">
+      <c r="Y23">
         <v>0</v>
       </c>
-      <c r="V23">
+      <c r="Z23">
         <v>2.8346994535519199E-2</v>
       </c>
-      <c r="W23">
+      <c r="AA23">
         <v>-2.0833333333333301E-2</v>
       </c>
-      <c r="X23">
+      <c r="AB23">
         <v>-7.5136612021858796E-3</v>
       </c>
-      <c r="Y23">
+      <c r="AC23">
         <v>3.3898305084745797E-2</v>
       </c>
+      <c r="AD23">
+        <f t="shared" si="6"/>
+        <v>2.459016393442625E-2</v>
+      </c>
+      <c r="AE23">
+        <f t="shared" si="12"/>
+        <v>3.77824858757062E-2</v>
+      </c>
+      <c r="AF23">
+        <f t="shared" si="7"/>
+        <v>3.7568306010929489E-3</v>
+      </c>
+      <c r="AG23">
+        <f t="shared" si="8"/>
+        <v>1.3192321941279958E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>25</v>
       </c>
@@ -2187,41 +2942,73 @@
       <c r="L24">
         <v>20.481005260081901</v>
       </c>
+      <c r="M24">
+        <f t="shared" si="10"/>
+        <v>1176.2033898305099</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="11"/>
+        <v>2411.7301875378098</v>
+      </c>
       <c r="O24">
+        <f t="shared" si="3"/>
+        <v>608.91623646321955</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="4"/>
+        <v>29.661703938396499</v>
+      </c>
+      <c r="S24">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P24">
+      <c r="T24">
         <v>3.125E-2</v>
       </c>
-      <c r="Q24">
+      <c r="U24">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="R24">
+      <c r="V24">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="S24">
+      <c r="W24">
         <v>4.91803278688525E-2</v>
       </c>
-      <c r="T24">
+      <c r="X24">
         <v>1.6949152542372801E-2</v>
       </c>
-      <c r="U24">
+      <c r="Y24">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="V24">
+      <c r="Z24">
         <v>2.8346994535519199E-2</v>
       </c>
-      <c r="W24">
+      <c r="AA24">
         <v>1.1953551912568401E-2</v>
       </c>
-      <c r="X24">
+      <c r="AB24">
         <v>-2.4180327868852498E-2</v>
       </c>
-      <c r="Y24">
+      <c r="AC24">
         <v>-1.5837732703528801E-2</v>
       </c>
+      <c r="AD24">
+        <f t="shared" si="6"/>
+        <v>4.0983606557377095E-2</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="12"/>
+        <v>2.0974576271186401E-2</v>
+      </c>
+      <c r="AF24">
+        <f t="shared" si="7"/>
+        <v>2.0150273224043801E-2</v>
+      </c>
+      <c r="AG24">
+        <f t="shared" si="8"/>
+        <v>-2.0009030286190652E-2</v>
+      </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>26</v>
       </c>
@@ -2258,41 +3045,73 @@
       <c r="L25">
         <v>388.41748438893802</v>
       </c>
+      <c r="M25">
+        <f t="shared" si="10"/>
+        <v>997.25735950044805</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="11"/>
+        <v>2507.12021343377</v>
+      </c>
       <c r="O25">
+        <f t="shared" si="3"/>
+        <v>357.692913811756</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>256.30274721644003</v>
+      </c>
+      <c r="S25">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P25">
+      <c r="T25">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="Q25">
+      <c r="U25">
         <v>1.5625E-2</v>
       </c>
-      <c r="R25">
+      <c r="V25">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="S25">
+      <c r="W25">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="T25">
+      <c r="X25">
         <v>8.4745762711864403E-2</v>
       </c>
-      <c r="U25">
+      <c r="Y25">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="V25">
+      <c r="Z25">
         <v>1.71618852459017E-2</v>
       </c>
-      <c r="W25">
+      <c r="AA25">
         <v>1.71618852459017E-2</v>
       </c>
-      <c r="X25">
+      <c r="AB25">
         <v>-7.7868852459016501E-3</v>
       </c>
-      <c r="Y25">
+      <c r="AC25">
         <v>5.19588774659627E-2</v>
       </c>
+      <c r="AD25">
+        <f t="shared" si="6"/>
+        <v>3.2786885245901697E-2</v>
+      </c>
+      <c r="AE25">
+        <f t="shared" si="12"/>
+        <v>5.4872881355932199E-2</v>
+      </c>
+      <c r="AF25">
+        <f t="shared" si="7"/>
+        <v>1.71618852459017E-2</v>
+      </c>
+      <c r="AG25">
+        <f t="shared" si="8"/>
+        <v>2.2085996110030523E-2</v>
+      </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>27</v>
       </c>
@@ -2329,41 +3148,73 @@
       <c r="L26">
         <v>148.971485411141</v>
       </c>
+      <c r="M26">
+        <f t="shared" si="10"/>
+        <v>1315.57899698341</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="11"/>
+        <v>2648.5095377842999</v>
+      </c>
       <c r="O26">
+        <f t="shared" si="3"/>
+        <v>475.45720598371099</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="4"/>
+        <v>8.6757719087409981</v>
+      </c>
+      <c r="S26">
         <v>6.25E-2</v>
       </c>
-      <c r="P26">
+      <c r="T26">
         <v>0.1875</v>
       </c>
-      <c r="Q26">
+      <c r="U26">
         <v>0.125</v>
       </c>
-      <c r="R26">
+      <c r="V26">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="S26">
+      <c r="W26">
         <v>1.63934426229508E-2</v>
       </c>
-      <c r="T26">
+      <c r="X26">
         <v>0.186440677966102</v>
       </c>
-      <c r="U26">
+      <c r="Y26">
         <v>9.8360655737704902E-2</v>
       </c>
-      <c r="V26">
+      <c r="Z26">
         <v>-0.108606557377049</v>
       </c>
-      <c r="W26">
+      <c r="AA26">
         <v>-2.6639344262295101E-2</v>
       </c>
-      <c r="X26">
+      <c r="AB26">
         <v>2.7322404371588098E-4</v>
       </c>
-      <c r="Y26">
+      <c r="AC26">
         <v>8.8080022228396698E-2</v>
       </c>
+      <c r="AD26">
+        <f t="shared" si="6"/>
+        <v>5.7377049180327849E-2</v>
+      </c>
+      <c r="AE26">
+        <f t="shared" si="12"/>
+        <v>0.10155367231638435</v>
+      </c>
+      <c r="AF26">
+        <f t="shared" si="7"/>
+        <v>-6.7622950819672054E-2</v>
+      </c>
+      <c r="AG26">
+        <f t="shared" si="8"/>
+        <v>4.4176623136056289E-2</v>
+      </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>28</v>
       </c>
@@ -2400,41 +3251,73 @@
       <c r="L27">
         <v>387.915951972556</v>
       </c>
+      <c r="M27">
+        <f t="shared" si="10"/>
+        <v>1333.79707792208</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="11"/>
+        <v>3112.13098693759</v>
+      </c>
       <c r="O27">
+        <f t="shared" si="3"/>
+        <v>655.38427870370947</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="4"/>
+        <v>222.26841554671751</v>
+      </c>
+      <c r="S27">
         <v>4.1666666666666602E-2</v>
       </c>
-      <c r="P27">
+      <c r="T27">
         <v>7.2916666666666602E-2</v>
       </c>
-      <c r="Q27">
+      <c r="U27">
         <v>5.7291666666666602E-2</v>
       </c>
-      <c r="R27">
+      <c r="V27">
         <v>9.1666666666666702E-2</v>
       </c>
-      <c r="S27">
+      <c r="W27">
         <v>0.114754098360656</v>
       </c>
-      <c r="T27">
+      <c r="X27">
         <v>0.11864406779661001</v>
       </c>
-      <c r="U27">
+      <c r="Y27">
         <v>8.1967213114754106E-2</v>
       </c>
-      <c r="V27">
+      <c r="Z27">
         <v>5.7462431693989097E-2</v>
       </c>
-      <c r="W27">
+      <c r="AA27">
         <v>2.46755464480874E-2</v>
       </c>
-      <c r="X27">
+      <c r="AB27">
         <v>-2.3087431693989101E-2</v>
       </c>
-      <c r="Y27">
+      <c r="AC27">
         <v>3.6676854681856101E-2</v>
       </c>
+      <c r="AD27">
+        <f t="shared" si="6"/>
+        <v>9.8360655737705055E-2</v>
+      </c>
+      <c r="AE27">
+        <f t="shared" si="12"/>
+        <v>0.10515536723163835</v>
+      </c>
+      <c r="AF27">
+        <f t="shared" si="7"/>
+        <v>4.1068989071038245E-2</v>
+      </c>
+      <c r="AG27">
+        <f t="shared" si="8"/>
+        <v>6.7947114939335002E-3</v>
+      </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>29</v>
       </c>
@@ -2471,41 +3354,73 @@
       <c r="L28">
         <v>121.241065830721</v>
       </c>
+      <c r="M28">
+        <f t="shared" si="10"/>
+        <v>1242.96933295647</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="11"/>
+        <v>2522.3808441558399</v>
+      </c>
       <c r="O28">
+        <f t="shared" si="3"/>
+        <v>645.3618626678475</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="4"/>
+        <v>18.221089121449502</v>
+      </c>
+      <c r="S28">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P28">
+      <c r="T28">
         <v>3.125E-2</v>
       </c>
-      <c r="Q28">
+      <c r="U28">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="R28">
+      <c r="V28">
         <v>0.05</v>
       </c>
-      <c r="S28">
+      <c r="W28">
         <v>8.1967213114754106E-2</v>
       </c>
-      <c r="T28">
+      <c r="X28">
         <v>5.0847457627118599E-2</v>
       </c>
-      <c r="U28">
+      <c r="Y28">
         <v>0</v>
       </c>
-      <c r="V28">
+      <c r="Z28">
         <v>6.1133879781420798E-2</v>
       </c>
-      <c r="W28">
+      <c r="AA28">
         <v>-2.0833333333333301E-2</v>
       </c>
-      <c r="X28">
+      <c r="AB28">
         <v>-3.1967213114753999E-2</v>
       </c>
-      <c r="Y28">
+      <c r="AC28">
         <v>5.0847457627118599E-2</v>
       </c>
+      <c r="AD28">
+        <f t="shared" si="6"/>
+        <v>4.0983606557377053E-2</v>
+      </c>
+      <c r="AE28">
+        <f t="shared" si="12"/>
+        <v>5.0423728813559304E-2</v>
+      </c>
+      <c r="AF28">
+        <f t="shared" si="7"/>
+        <v>2.0150273224043749E-2</v>
+      </c>
+      <c r="AG28">
+        <f t="shared" si="8"/>
+        <v>9.4401222561822998E-3</v>
+      </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>30</v>
       </c>
@@ -2542,41 +3457,73 @@
       <c r="L29">
         <v>241.600250626567</v>
       </c>
+      <c r="M29">
+        <f t="shared" si="10"/>
+        <v>1778.513227513225</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="11"/>
+        <v>3656.3859649122801</v>
+      </c>
       <c r="O29">
+        <f t="shared" si="3"/>
+        <v>1137.5281265031249</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="4"/>
+        <v>49.679754942913007</v>
+      </c>
+      <c r="S29">
         <v>6.25E-2</v>
       </c>
-      <c r="P29">
+      <c r="T29">
         <v>6.25E-2</v>
       </c>
-      <c r="Q29">
+      <c r="U29">
         <v>6.25E-2</v>
       </c>
-      <c r="R29">
+      <c r="V29">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="S29">
+      <c r="W29">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="T29">
+      <c r="X29">
         <v>5.0847457627118599E-2</v>
       </c>
-      <c r="U29">
+      <c r="Y29">
         <v>3.2786885245901697E-2</v>
       </c>
-      <c r="V29">
+      <c r="Z29">
         <v>-2.97131147540983E-2</v>
       </c>
-      <c r="W29">
+      <c r="AA29">
         <v>-2.97131147540983E-2</v>
       </c>
-      <c r="X29">
+      <c r="AB29">
         <v>-1.6120218579234999E-2</v>
       </c>
-      <c r="Y29">
+      <c r="AC29">
         <v>1.8060572381216899E-2</v>
       </c>
+      <c r="AD29">
+        <f t="shared" si="6"/>
+        <v>3.2786885245901697E-2</v>
+      </c>
+      <c r="AE29">
+        <f t="shared" si="12"/>
+        <v>3.3757062146892648E-2</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" si="7"/>
+        <v>-2.97131147540983E-2</v>
+      </c>
+      <c r="AG29">
+        <f t="shared" si="8"/>
+        <v>9.7017690099094993E-4</v>
+      </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>31</v>
       </c>
@@ -2613,41 +3560,73 @@
       <c r="L30">
         <v>267.49765807962501</v>
       </c>
+      <c r="M30">
+        <f t="shared" si="10"/>
+        <v>1344.0872365339551</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="11"/>
+        <v>2920.3227812323403</v>
+      </c>
       <c r="O30">
+        <f t="shared" si="3"/>
+        <v>696.68197337606352</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="4"/>
+        <v>116.0741540822093</v>
+      </c>
+      <c r="S30">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="P30">
+      <c r="T30">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="Q30">
+      <c r="U30">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="R30">
+      <c r="V30">
         <v>8.4033613445377905E-3</v>
       </c>
-      <c r="S30">
+      <c r="W30">
         <v>0</v>
       </c>
-      <c r="T30">
+      <c r="X30">
         <v>1.6949152542372801E-2</v>
       </c>
-      <c r="U30">
+      <c r="Y30">
         <v>0</v>
       </c>
-      <c r="V30">
+      <c r="Z30">
         <v>-1.04166666666666E-2</v>
       </c>
-      <c r="W30">
+      <c r="AA30">
         <v>-1.04166666666666E-2</v>
       </c>
-      <c r="X30">
+      <c r="AB30">
         <v>8.4033613445377905E-3</v>
       </c>
-      <c r="Y30">
+      <c r="AC30">
         <v>1.6949152542372801E-2</v>
       </c>
+      <c r="AD30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AE30">
+        <f t="shared" si="12"/>
+        <v>1.2676256943455297E-2</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="7"/>
+        <v>-1.04166666666666E-2</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="8"/>
+        <v>1.2676256943455297E-2</v>
+      </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>36</v>
       </c>
@@ -2684,317 +3663,647 @@
       <c r="L31">
         <v>120.88196125908</v>
       </c>
+      <c r="M31">
+        <f t="shared" si="10"/>
+        <v>1496.3047820823249</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="11"/>
+        <v>3102.98116760829</v>
+      </c>
       <c r="O31">
+        <f t="shared" si="3"/>
+        <v>729.88994445634501</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>55.185801721818699</v>
+      </c>
+      <c r="S31">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="P31">
+      <c r="T31">
         <v>1.04166666666666E-2</v>
       </c>
-      <c r="Q31">
+      <c r="U31">
         <v>1.5625E-2</v>
       </c>
-      <c r="R31">
+      <c r="V31">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="S31">
+      <c r="W31">
         <v>1.63934426229508E-2</v>
       </c>
-      <c r="T31">
+      <c r="X31">
         <v>3.3898305084745797E-2</v>
       </c>
-      <c r="U31">
+      <c r="Y31">
         <v>1.63934426229508E-2</v>
       </c>
-      <c r="V31">
+      <c r="Z31">
         <v>7.6844262295083798E-4</v>
       </c>
-      <c r="W31">
+      <c r="AA31">
         <v>7.6844262295083798E-4</v>
       </c>
-      <c r="X31">
+      <c r="AB31">
         <v>8.6065573770491809E-3</v>
       </c>
-      <c r="Y31">
+      <c r="AC31">
         <v>1.75048624617949E-2</v>
       </c>
+      <c r="AD31">
+        <f t="shared" si="6"/>
+        <v>1.63934426229508E-2</v>
+      </c>
+      <c r="AE31">
+        <f t="shared" si="12"/>
+        <v>2.9449152542372899E-2</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="7"/>
+        <v>7.6844262295083798E-4</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="8"/>
+        <v>1.3055709919422041E-2</v>
+      </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>12</v>
       </c>
       <c r="B33">
-        <f>AVERAGE(B2:B31)</f>
+        <f t="shared" ref="B33:L33" si="13">AVERAGE(B2:B31)</f>
         <v>678.61222136344941</v>
       </c>
       <c r="C33">
-        <f>AVERAGE(C2:C31)</f>
+        <f t="shared" si="13"/>
         <v>758.34979134793434</v>
       </c>
       <c r="D33">
-        <f>AVERAGE(D2:D31)</f>
+        <f t="shared" si="13"/>
         <v>718.48100635569176</v>
       </c>
       <c r="E33">
-        <f>AVERAGE(E2:E31)</f>
+        <f t="shared" si="13"/>
         <v>1465.0243804717741</v>
       </c>
       <c r="F33">
-        <f>AVERAGE(F2:F31)</f>
+        <f t="shared" si="13"/>
         <v>1415.3772511468139</v>
       </c>
       <c r="G33">
-        <f>AVERAGE(G2:G31)</f>
+        <f t="shared" si="13"/>
         <v>1548.2124582343722</v>
       </c>
       <c r="H33">
-        <f>AVERAGE(H2:H31)</f>
+        <f t="shared" si="13"/>
         <v>1338.0325337956574</v>
       </c>
       <c r="I33">
-        <f>AVERAGE(I2:I31)</f>
+        <f t="shared" si="13"/>
         <v>696.89624479112297</v>
       </c>
       <c r="J33">
-        <f>AVERAGE(J2:J31)</f>
+        <f t="shared" si="13"/>
         <v>619.55152743996541</v>
       </c>
       <c r="K33">
-        <f>AVERAGE(K2:K31)</f>
+        <f t="shared" si="13"/>
         <v>49.64712932495916</v>
       </c>
       <c r="L33">
-        <f>AVERAGE(L2:L31)</f>
+        <f t="shared" si="13"/>
         <v>210.17992443871418</v>
       </c>
+      <c r="M33">
+        <f t="shared" ref="M33:N33" si="14">AVERAGE(M2:M31)</f>
+        <v>1376.704892471236</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="14"/>
+        <v>2269.6096230763405</v>
+      </c>
       <c r="O33">
-        <f>AVERAGE(O2:O31)</f>
+        <f t="shared" ref="O33:P33" si="15">AVERAGE(O2:O31)</f>
+        <v>658.22388611554425</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="15"/>
+        <v>129.91352688183667</v>
+      </c>
+      <c r="S33">
+        <f t="shared" ref="S33:AE33" si="16">AVERAGE(S2:S31)</f>
         <v>1.9820984198083844E-2</v>
       </c>
-      <c r="P33">
-        <f>AVERAGE(P2:P31)</f>
+      <c r="T33">
+        <f t="shared" si="16"/>
         <v>4.3530496418949988E-2</v>
       </c>
-      <c r="Q33">
-        <f>AVERAGE(Q2:Q31)</f>
+      <c r="U33">
+        <f t="shared" si="16"/>
         <v>3.1675740308516914E-2</v>
       </c>
-      <c r="R33">
-        <f>AVERAGE(R2:R31)</f>
+      <c r="V33">
+        <f t="shared" si="16"/>
         <v>3.5941737260689874E-2</v>
       </c>
-      <c r="S33">
-        <f>AVERAGE(S2:S31)</f>
+      <c r="W33">
+        <f t="shared" si="16"/>
         <v>4.6696128983661371E-2</v>
       </c>
-      <c r="T33">
-        <f>AVERAGE(T2:T31)</f>
+      <c r="X33">
+        <f t="shared" si="16"/>
         <v>5.1641032627956877E-2</v>
       </c>
-      <c r="U33">
-        <f>AVERAGE(U2:U31)</f>
+      <c r="Y33">
+        <f t="shared" si="16"/>
         <v>2.4821619245022304E-2</v>
       </c>
-      <c r="V33">
-        <f>AVERAGE(V2:V31)</f>
+      <c r="Z33">
+        <f t="shared" si="16"/>
         <v>1.5020388675144448E-2</v>
       </c>
-      <c r="W33">
-        <f>AVERAGE(W2:W31)</f>
+      <c r="AA33">
+        <f t="shared" si="16"/>
         <v>-6.8541210634946153E-3</v>
       </c>
-      <c r="X33">
-        <f>AVERAGE(X2:X31)</f>
+      <c r="AB33">
+        <f t="shared" si="16"/>
         <v>-1.0754391722971466E-2</v>
       </c>
-      <c r="Y33">
-        <f>AVERAGE(Y2:Y31)</f>
+      <c r="AC33">
+        <f t="shared" si="16"/>
         <v>2.6819413382934573E-2</v>
       </c>
+      <c r="AD33">
+        <f t="shared" si="16"/>
+        <v>3.5758874114341831E-2</v>
+      </c>
+      <c r="AE33">
+        <f t="shared" si="16"/>
+        <v>4.3791384944323372E-2</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" ref="AF33:AG33" si="17">AVERAGE(AF2:AF31)</f>
+        <v>4.0831338058249182E-3</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" si="17"/>
+        <v>8.0325108299815519E-3</v>
+      </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>13</v>
       </c>
       <c r="B34">
-        <f>STDEV(B2:B31)</f>
+        <f t="shared" ref="B34:L34" si="18">STDEV(B2:B31)</f>
         <v>121.95311455974404</v>
       </c>
       <c r="C34">
-        <f>STDEV(C2:C31)</f>
+        <f t="shared" si="18"/>
         <v>176.85980032972546</v>
       </c>
       <c r="D34">
-        <f>STDEV(D2:D31)</f>
+        <f t="shared" si="18"/>
         <v>136.69038852516829</v>
       </c>
       <c r="E34">
-        <f>STDEV(E2:E31)</f>
+        <f t="shared" si="18"/>
         <v>273.35310379791241</v>
       </c>
       <c r="F34">
-        <f>STDEV(F2:F31)</f>
+        <f t="shared" si="18"/>
         <v>296.56752707437886</v>
       </c>
       <c r="G34">
-        <f>STDEV(G2:G31)</f>
+        <f t="shared" si="18"/>
         <v>400.94432554237142</v>
       </c>
       <c r="H34">
-        <f>STDEV(H2:H31)</f>
+        <f t="shared" si="18"/>
         <v>330.98491113393413</v>
       </c>
       <c r="I34">
-        <f>STDEV(I2:I31)</f>
+        <f t="shared" si="18"/>
         <v>239.25829917623767</v>
       </c>
       <c r="J34">
-        <f>STDEV(J2:J31)</f>
+        <f t="shared" si="18"/>
         <v>273.0930605798481</v>
       </c>
       <c r="K34">
-        <f>STDEV(K2:K31)</f>
+        <f t="shared" si="18"/>
         <v>136.01665571746932</v>
       </c>
       <c r="L34">
-        <f>STDEV(L2:L31)</f>
+        <f t="shared" si="18"/>
         <v>141.18086876605688</v>
       </c>
+      <c r="M34">
+        <f t="shared" ref="M34:N34" si="19">STDEV(M2:M31)</f>
+        <v>297.24089964575575</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="19"/>
+        <v>1134.9119020279509</v>
+      </c>
       <c r="O34">
-        <f>STDEV(O2:O31)</f>
+        <f t="shared" ref="O34:P34" si="20">STDEV(O2:O31)</f>
+        <v>235.61127816030213</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="20"/>
+        <v>96.94307985734396</v>
+      </c>
+      <c r="S34">
+        <f t="shared" ref="S34:AE34" si="21">STDEV(S2:S31)</f>
         <v>2.1450290599638638E-2</v>
       </c>
-      <c r="P34">
-        <f>STDEV(P2:P31)</f>
+      <c r="T34">
+        <f t="shared" si="21"/>
         <v>4.0789593497577555E-2</v>
       </c>
-      <c r="Q34">
-        <f>STDEV(Q2:Q31)</f>
+      <c r="U34">
+        <f t="shared" si="21"/>
         <v>2.5619369468777478E-2</v>
       </c>
-      <c r="R34">
-        <f>STDEV(R2:R31)</f>
+      <c r="V34">
+        <f t="shared" si="21"/>
         <v>3.0001981098578594E-2</v>
       </c>
-      <c r="S34">
-        <f>STDEV(S2:S31)</f>
+      <c r="W34">
+        <f t="shared" si="21"/>
         <v>4.2292865842371546E-2</v>
       </c>
-      <c r="T34">
-        <f>STDEV(T2:T31)</f>
+      <c r="X34">
+        <f t="shared" si="21"/>
         <v>4.3381064891508336E-2</v>
       </c>
-      <c r="U34">
-        <f>STDEV(U2:U31)</f>
+      <c r="Y34">
+        <f t="shared" si="21"/>
         <v>2.6380588360491727E-2</v>
       </c>
-      <c r="V34">
-        <f>STDEV(V2:V31)</f>
+      <c r="Z34">
+        <f t="shared" si="21"/>
         <v>4.567379815332024E-2</v>
       </c>
-      <c r="W34">
-        <f>STDEV(W2:W31)</f>
+      <c r="AA34">
+        <f t="shared" si="21"/>
         <v>2.0315347984632786E-2</v>
       </c>
-      <c r="X34">
-        <f>STDEV(X2:X31)</f>
+      <c r="AB34">
+        <f t="shared" si="21"/>
         <v>2.1497598742435602E-2</v>
       </c>
-      <c r="Y34">
-        <f>STDEV(Y2:Y31)</f>
+      <c r="AC34">
+        <f t="shared" si="21"/>
         <v>3.0625475067053026E-2</v>
       </c>
+      <c r="AD34">
+        <f t="shared" si="21"/>
+        <v>2.8311154716433199E-2</v>
+      </c>
+      <c r="AE34">
+        <f t="shared" si="21"/>
+        <v>3.1998585414306245E-2</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" ref="AF34:AG34" si="22">STDEV(AF2:AF31)</f>
+        <v>2.8436158503180837E-2</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="22"/>
+        <v>1.984956440313361E-2</v>
+      </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
       <c r="B35">
-        <f>B34/SQRT(31)</f>
+        <f t="shared" ref="B35:L35" si="23">B34/SQRT(31)</f>
         <v>21.903425973608709</v>
       </c>
       <c r="C35">
-        <f>C34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>31.764957854615446</v>
       </c>
       <c r="D35">
-        <f>D34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>24.550318515220059</v>
       </c>
       <c r="E35">
-        <f>E34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>49.095666767580411</v>
       </c>
       <c r="F35">
-        <f>F34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>53.265100271527558</v>
       </c>
       <c r="G35">
-        <f>G34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>72.011726684959186</v>
       </c>
       <c r="H35">
-        <f>H34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>59.446644930515497</v>
       </c>
       <c r="I35">
-        <f>I34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>42.972059085960638</v>
       </c>
       <c r="J35">
-        <f>J34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>49.048961626859956</v>
       </c>
       <c r="K35">
-        <f>K34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>24.429312530807938</v>
       </c>
       <c r="L35">
-        <f>L34/SQRT(31)</f>
+        <f t="shared" si="23"/>
         <v>25.356832575130117</v>
       </c>
+      <c r="M35">
+        <f t="shared" ref="M35" si="24">M34/SQRT(31)</f>
+        <v>53.386041555586253</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ref="N35" si="25">N34/SQRT(31)</f>
+        <v>203.83619493751169</v>
+      </c>
       <c r="O35">
-        <f>O34/SQRT(30)</f>
+        <f t="shared" ref="O35" si="26">O34/SQRT(31)</f>
+        <v>42.317034774895539</v>
+      </c>
+      <c r="P35">
+        <f t="shared" ref="P35" si="27">P34/SQRT(31)</f>
+        <v>17.411491137184022</v>
+      </c>
+      <c r="S35">
+        <f t="shared" ref="S35:AC35" si="28">S34/SQRT(30)</f>
         <v>3.9162693421543656E-3</v>
       </c>
-      <c r="P35">
-        <f>P34/SQRT(30)</f>
+      <c r="T35">
+        <f t="shared" si="28"/>
         <v>7.4471268233630905E-3</v>
       </c>
-      <c r="Q35">
-        <f>Q34/SQRT(30)</f>
+      <c r="U35">
+        <f t="shared" si="28"/>
         <v>4.6774355223695233E-3</v>
       </c>
-      <c r="R35">
-        <f>R34/SQRT(30)</f>
+      <c r="V35">
+        <f t="shared" si="28"/>
         <v>5.4775872725117067E-3</v>
       </c>
-      <c r="S35">
-        <f>S34/SQRT(30)</f>
+      <c r="W35">
+        <f t="shared" si="28"/>
         <v>7.7215855478022085E-3</v>
       </c>
-      <c r="T35">
-        <f>T34/SQRT(30)</f>
+      <c r="X35">
+        <f t="shared" si="28"/>
         <v>7.920262603224839E-3</v>
       </c>
-      <c r="U35">
-        <f>U34/SQRT(30)</f>
+      <c r="Y35">
+        <f t="shared" si="28"/>
         <v>4.8164144417665155E-3</v>
       </c>
-      <c r="V35">
-        <f>V34/SQRT(30)</f>
+      <c r="Z35">
+        <f t="shared" si="28"/>
         <v>8.3388565118370974E-3</v>
       </c>
-      <c r="W35">
-        <f>W34/SQRT(30)</f>
+      <c r="AA35">
+        <f t="shared" si="28"/>
         <v>3.7090581182501639E-3</v>
       </c>
-      <c r="X35">
-        <f>X34/SQRT(30)</f>
+      <c r="AB35">
+        <f t="shared" si="28"/>
         <v>3.9249065878088907E-3</v>
       </c>
-      <c r="Y35">
-        <f>Y34/SQRT(30)</f>
+      <c r="AC35">
+        <f t="shared" si="28"/>
         <v>5.5914211761789942E-3</v>
+      </c>
+      <c r="AD35">
+        <f t="shared" ref="AD35" si="29">AD34/SQRT(30)</f>
+        <v>5.1688860224030795E-3</v>
+      </c>
+      <c r="AE35">
+        <f t="shared" ref="AE35" si="30">AE34/SQRT(30)</f>
+        <v>5.842115679890441E-3</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" ref="AF35" si="31">AF34/SQRT(30)</f>
+        <v>5.1917084869948279E-3</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" ref="AG35" si="32">AG34/SQRT(30)</f>
+        <v>3.6240180600826156E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36">
+        <f>(B33 +1.96*(B35))</f>
+        <v>721.54293627172251</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:L36" si="33">(C33 +1.96*(C35))</f>
+        <v>820.60910874298065</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="33"/>
+        <v>766.59963064552312</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="33"/>
+        <v>1561.2518873362317</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="33"/>
+        <v>1519.7768476790079</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="33"/>
+        <v>1689.3554425368923</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="33"/>
+        <v>1454.5479578594677</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="33"/>
+        <v>781.12148059960577</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="33"/>
+        <v>715.68749222861095</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="33"/>
+        <v>97.528581885342717</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="33"/>
+        <v>259.8793162859692</v>
+      </c>
+      <c r="S36">
+        <f t="shared" ref="S36:AE36" si="34">(S33 +1.96*(S35))</f>
+        <v>2.74968721087064E-2</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="34"/>
+        <v>5.8126864992741646E-2</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="34"/>
+        <v>4.0843513932361179E-2</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="34"/>
+        <v>4.6677808314812816E-2</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="34"/>
+        <v>6.1830436657353702E-2</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="34"/>
+        <v>6.7164747330277566E-2</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="34"/>
+        <v>3.4261791550884671E-2</v>
+      </c>
+      <c r="Z36">
+        <f t="shared" si="34"/>
+        <v>3.1364547438345158E-2</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" si="34"/>
+        <v>4.1563284827570574E-4</v>
+      </c>
+      <c r="AB36">
+        <f t="shared" si="34"/>
+        <v>-3.0615748108660402E-3</v>
+      </c>
+      <c r="AC36">
+        <f t="shared" si="34"/>
+        <v>3.7778598888245404E-2</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" si="34"/>
+        <v>4.5889890718251863E-2</v>
+      </c>
+      <c r="AE36">
+        <f t="shared" si="34"/>
+        <v>5.5241931676908634E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37">
+        <f>(B33 -1.96*(B35))</f>
+        <v>635.6815064551763</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ref="C37:L37" si="35">(C33 -1.96*(C35))</f>
+        <v>696.09047395288803</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="35"/>
+        <v>670.3623820658604</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="35"/>
+        <v>1368.7968736073165</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="35"/>
+        <v>1310.97765461462</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="35"/>
+        <v>1407.0694739318521</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="35"/>
+        <v>1221.5171097318471</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="35"/>
+        <v>612.67100898264016</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="35"/>
+        <v>523.41556265131987</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="35"/>
+        <v>1.765676764575602</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="35"/>
+        <v>160.48053259145917</v>
+      </c>
+      <c r="S37">
+        <f t="shared" ref="S37:AE37" si="36">(S33 -1.96*(S35))</f>
+        <v>1.2145096287461288E-2</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="36"/>
+        <v>2.8934127845158329E-2</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="36"/>
+        <v>2.2507966684672649E-2</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="36"/>
+        <v>2.5205666206566928E-2</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="36"/>
+        <v>3.156182130996904E-2</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="36"/>
+        <v>3.6117317925636196E-2</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="36"/>
+        <v>1.5381446939159934E-2</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" si="36"/>
+        <v>-1.3237700880562638E-3</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" si="36"/>
+        <v>-1.4123874975264936E-2</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="36"/>
+        <v>-1.8447208635076894E-2</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" si="36"/>
+        <v>1.5860227877623746E-2</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="36"/>
+        <v>2.5627857510431794E-2</v>
+      </c>
+      <c r="AE37">
+        <f t="shared" si="36"/>
+        <v>3.234083821173811E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>